<commit_message>
first big update: from chatgpt prototype to better structured code
</commit_message>
<xml_diff>
--- a/your_file.xlsx
+++ b/your_file.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zocher\Documents\Sonstiges\Maria\Dashboad_Demo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zocher\Documents\Smartgit\Lmnn_Demo_Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BECEDA33-A257-4EA8-A649-193C51ECF709}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D7A538-8861-44C2-88A2-15B493C1D03D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>Time</t>
   </si>
@@ -51,16 +51,7 @@
     <t>0.26</t>
   </si>
   <si>
-    <t>0.24</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
     <t>0.35</t>
-  </si>
-  <si>
-    <t>0.44</t>
   </si>
   <si>
     <t>0.53</t>
@@ -416,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1441"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A781" workbookViewId="0">
-      <selection activeCell="E792" sqref="E792"/>
+    <sheetView tabSelected="1" topLeftCell="A1417" workbookViewId="0">
+      <selection activeCell="E725" sqref="E725"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,7 +426,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -738,7 +729,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -2556,7 +2547,7 @@
         <v>421</v>
       </c>
       <c r="B422" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="423" spans="1:2" x14ac:dyDescent="0.3">
@@ -2859,7 +2850,7 @@
         <v>481</v>
       </c>
       <c r="B482" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="483" spans="1:2" x14ac:dyDescent="0.3">
@@ -3162,7 +3153,7 @@
         <v>541</v>
       </c>
       <c r="B542" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="543" spans="1:2" x14ac:dyDescent="0.3">
@@ -3465,7 +3456,7 @@
         <v>601</v>
       </c>
       <c r="B602" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="603" spans="1:2" x14ac:dyDescent="0.3">
@@ -3768,7 +3759,7 @@
         <v>661</v>
       </c>
       <c r="B662" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="663" spans="1:2" x14ac:dyDescent="0.3">
@@ -4071,7 +4062,7 @@
         <v>721</v>
       </c>
       <c r="B722" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.3">
@@ -4374,7 +4365,7 @@
         <v>781</v>
       </c>
       <c r="B782" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.3">
@@ -4677,7 +4668,7 @@
         <v>841</v>
       </c>
       <c r="B842" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.3">
@@ -4980,7 +4971,7 @@
         <v>901</v>
       </c>
       <c r="B902" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="903" spans="1:2" x14ac:dyDescent="0.3">
@@ -5278,7 +5269,7 @@
         <v>960</v>
       </c>
       <c r="B961" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="962" spans="1:2" x14ac:dyDescent="0.3">
@@ -5586,7 +5577,7 @@
         <v>1021</v>
       </c>
       <c r="B1022" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="1023" spans="1:2" x14ac:dyDescent="0.3">
@@ -5889,7 +5880,7 @@
         <v>1081</v>
       </c>
       <c r="B1082" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="1083" spans="1:2" x14ac:dyDescent="0.3">
@@ -6192,7 +6183,7 @@
         <v>1141</v>
       </c>
       <c r="B1142" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="1143" spans="1:2" x14ac:dyDescent="0.3">
@@ -6495,7 +6486,7 @@
         <v>1201</v>
       </c>
       <c r="B1202" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="1203" spans="1:2" x14ac:dyDescent="0.3">
@@ -6798,7 +6789,7 @@
         <v>1261</v>
       </c>
       <c r="B1262" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="1263" spans="1:2" x14ac:dyDescent="0.3">
@@ -7101,7 +7092,7 @@
         <v>1321</v>
       </c>
       <c r="B1322" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="1323" spans="1:2" x14ac:dyDescent="0.3">
@@ -7404,7 +7395,7 @@
         <v>1381</v>
       </c>
       <c r="B1382" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="1383" spans="1:2" x14ac:dyDescent="0.3">
@@ -7702,7 +7693,7 @@
         <v>1440</v>
       </c>
       <c r="B1441" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>